<commit_message>
Fixed Faculty and student upload functions, and added appropriate images and guidelines to the upload pages.
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/1facultyUpload.xlsx
+++ b/data/InOrderUploadTests/1facultyUpload.xlsx
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-enable unit tests in CI.
Properly migrate to cypress session, away from deprecated preserveOnce.

In several cases, comment tests for functionality that is clearly not working.

In a few, open an issue.

In several, address light bit rot, such as stale test inputs.

Fix one actual bug in admin form behavior in the grad tracking app.

CS 01 has a hack that broke the test for CS 13. There is probably a cleaner way to deal with this, but I replicated the code for now.
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/1facultyUpload.xlsx
+++ b/data/InOrderUploadTests/1facultyUpload.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donimal/CS-Grad-Tracking/data/InOrderUploadTests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75CD07D-2980-EB4A-876C-73E6FEF2F6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Faculty" sheetId="1" r:id="rId4"/>
+    <sheet name="Faculty" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi5cQI9S19k8ui67iZD/bQrLM99VA=="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="255">
   <si>
     <t>onyen</t>
   </si>
@@ -778,76 +787,92 @@
   </si>
   <si>
     <t>Yap</t>
+  </si>
+  <si>
+    <t>directorOfGraduateStudies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1037,17 +1062,22 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +1105,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="J1" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1093,16 +1126,19 @@
         <v>12</v>
       </c>
       <c r="F2" s="1">
-        <v>7.2004693E8</v>
+        <v>720046930</v>
       </c>
       <c r="G2" s="1">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="J2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1119,16 +1155,19 @@
         <v>17</v>
       </c>
       <c r="F3" s="1">
-        <v>7.04273269E8</v>
+        <v>704273269</v>
       </c>
       <c r="G3" s="1">
-        <v>126.0</v>
+        <v>126</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="J3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1145,16 +1184,19 @@
         <v>21</v>
       </c>
       <c r="F4" s="1">
-        <v>7.14730206E8</v>
+        <v>714730206</v>
       </c>
       <c r="G4" s="1">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="J4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1171,16 +1213,19 @@
         <v>26</v>
       </c>
       <c r="F5" s="1">
-        <v>7.04290844E8</v>
+        <v>704290844</v>
       </c>
       <c r="G5" s="1">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="J5" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1197,16 +1242,19 @@
         <v>31</v>
       </c>
       <c r="F6" s="1">
-        <v>7.30139106E8</v>
+        <v>730139106</v>
       </c>
       <c r="G6" s="1">
-        <v>139.0</v>
+        <v>139</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1223,16 +1271,19 @@
         <v>36</v>
       </c>
       <c r="F7" s="1">
-        <v>7.20365853E8</v>
+        <v>720365853</v>
       </c>
       <c r="G7" s="1">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -1249,16 +1300,19 @@
         <v>40</v>
       </c>
       <c r="F8" s="1">
-        <v>7.01876731E8</v>
+        <v>701876731</v>
       </c>
       <c r="G8" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="J8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1275,16 +1329,19 @@
         <v>44</v>
       </c>
       <c r="F9" s="1">
-        <v>7.20451068E8</v>
+        <v>720451068</v>
       </c>
       <c r="G9" s="1">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -1301,16 +1358,19 @@
         <v>49</v>
       </c>
       <c r="F10" s="1">
-        <v>7.14338468E8</v>
+        <v>714338468</v>
       </c>
       <c r="G10" s="1">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="J10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1327,16 +1387,19 @@
         <v>53</v>
       </c>
       <c r="F11" s="1">
-        <v>7.30291808E8</v>
+        <v>730291808</v>
       </c>
       <c r="G11" s="1">
-        <v>148.0</v>
+        <v>148</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="J11" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -1353,16 +1416,19 @@
         <v>57</v>
       </c>
       <c r="F12" s="1">
-        <v>7.04279085E8</v>
+        <v>704279085</v>
       </c>
       <c r="G12" s="1">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="J12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -1379,16 +1445,19 @@
         <v>61</v>
       </c>
       <c r="F13" s="1">
-        <v>7.30300195E8</v>
+        <v>730300195</v>
       </c>
       <c r="G13" s="1">
-        <v>144.0</v>
+        <v>144</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="J13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -1405,16 +1474,19 @@
         <v>65</v>
       </c>
       <c r="F14" s="1">
-        <v>7.13281075E8</v>
+        <v>713281075</v>
       </c>
       <c r="G14" s="1">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="J14" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -1431,16 +1503,19 @@
         <v>70</v>
       </c>
       <c r="F15" s="1">
-        <v>7.11856002E8</v>
+        <v>711856002</v>
       </c>
       <c r="G15" s="1">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="J15" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
@@ -1457,16 +1532,19 @@
         <v>74</v>
       </c>
       <c r="F16" s="1">
-        <v>7.04288472E8</v>
+        <v>704288472</v>
       </c>
       <c r="G16" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="J16" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -1483,16 +1561,19 @@
         <v>78</v>
       </c>
       <c r="F17" s="1">
-        <v>7.11837205E8</v>
+        <v>711837205</v>
       </c>
       <c r="G17" s="1">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="J17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
@@ -1509,16 +1590,19 @@
         <v>82</v>
       </c>
       <c r="F18" s="1">
-        <v>7.04275348E8</v>
+        <v>704275348</v>
       </c>
       <c r="G18" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="J18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>83</v>
       </c>
@@ -1535,16 +1619,19 @@
         <v>87</v>
       </c>
       <c r="F19" s="1">
-        <v>7.10453084E8</v>
+        <v>710453084</v>
       </c>
       <c r="G19" s="1">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
+      <c r="J19" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
@@ -1561,10 +1648,10 @@
         <v>91</v>
       </c>
       <c r="F20" s="1">
-        <v>7.10233624E8</v>
+        <v>710233624</v>
       </c>
       <c r="G20" s="1">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="H20" s="1" t="b">
         <v>1</v>
@@ -1572,8 +1659,11 @@
       <c r="I20" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
+      <c r="J20" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -1590,10 +1680,10 @@
         <v>96</v>
       </c>
       <c r="F21" s="1">
-        <v>7.1175834E8</v>
+        <v>711758340</v>
       </c>
       <c r="G21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1" t="b">
         <v>1</v>
@@ -1601,8 +1691,11 @@
       <c r="I21" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+      <c r="J21" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
@@ -1619,42 +1712,48 @@
         <v>100</v>
       </c>
       <c r="F22" s="1">
-        <v>7.20441075E8</v>
+        <v>720441075</v>
       </c>
       <c r="G22" s="1">
-        <v>137.0</v>
+        <v>137</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="J22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F23" s="1">
-        <v>7.01534022E8</v>
+        <v>701534022</v>
       </c>
       <c r="G23" s="1">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
+      <c r="J23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>105</v>
       </c>
@@ -1671,16 +1770,19 @@
         <v>108</v>
       </c>
       <c r="F24" s="1">
-        <v>7.20176068E8</v>
+        <v>720176068</v>
       </c>
       <c r="G24" s="1">
-        <v>147.0</v>
+        <v>147</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
+      <c r="J24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
@@ -1697,16 +1799,19 @@
         <v>112</v>
       </c>
       <c r="F25" s="1">
-        <v>7.04274598E8</v>
+        <v>704274598</v>
       </c>
       <c r="G25" s="1">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
+      <c r="J25" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>113</v>
       </c>
@@ -1723,16 +1828,19 @@
         <v>116</v>
       </c>
       <c r="F26" s="1">
-        <v>7.07696375E8</v>
+        <v>707696375</v>
       </c>
       <c r="G26" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+      <c r="J26" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>117</v>
       </c>
@@ -1749,16 +1857,19 @@
         <v>120</v>
       </c>
       <c r="F27" s="1">
-        <v>7.03745132E8</v>
+        <v>703745132</v>
       </c>
       <c r="G27" s="1">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+      <c r="J27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>121</v>
       </c>
@@ -1775,16 +1886,19 @@
         <v>125</v>
       </c>
       <c r="F28" s="1">
-        <v>7.146349E8</v>
+        <v>714634900</v>
       </c>
       <c r="G28" s="1">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+      <c r="J28" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>126</v>
       </c>
@@ -1801,16 +1915,19 @@
         <v>130</v>
       </c>
       <c r="F29" s="1">
-        <v>7.05472186E8</v>
+        <v>705472186</v>
       </c>
       <c r="G29" s="1">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>131</v>
       </c>
@@ -1827,16 +1944,19 @@
         <v>134</v>
       </c>
       <c r="F30" s="1">
-        <v>7.1407717E8</v>
+        <v>714077170</v>
       </c>
       <c r="G30" s="1">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="I30" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
+      <c r="J30" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>135</v>
       </c>
@@ -1853,16 +1973,19 @@
         <v>138</v>
       </c>
       <c r="F31" s="1">
-        <v>7.30064202E8</v>
+        <v>730064202</v>
       </c>
       <c r="G31" s="1">
-        <v>136.0</v>
+        <v>136</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>139</v>
       </c>
@@ -1879,16 +2002,19 @@
         <v>142</v>
       </c>
       <c r="F32" s="1">
-        <v>7.10990354E8</v>
+        <v>710990354</v>
       </c>
       <c r="G32" s="1">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
+      <c r="J32" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>143</v>
       </c>
@@ -1905,16 +2031,19 @@
         <v>146</v>
       </c>
       <c r="F33" s="1">
-        <v>7.30295982E8</v>
+        <v>730295982</v>
       </c>
       <c r="G33" s="1">
-        <v>142.0</v>
+        <v>142</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
+      <c r="J33" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>147</v>
       </c>
@@ -1931,16 +2060,19 @@
         <v>151</v>
       </c>
       <c r="F34" s="1">
-        <v>7.04208957E8</v>
+        <v>704208957</v>
       </c>
       <c r="G34" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+      <c r="J34" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>152</v>
       </c>
@@ -1957,16 +2089,19 @@
         <v>155</v>
       </c>
       <c r="F35" s="1">
-        <v>7.04213001E8</v>
+        <v>704213001</v>
       </c>
       <c r="G35" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="I35" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
+      <c r="J35" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>156</v>
       </c>
@@ -1983,16 +2118,19 @@
         <v>159</v>
       </c>
       <c r="F36" s="1">
-        <v>7.01569707E8</v>
+        <v>701569707</v>
       </c>
       <c r="G36" s="1">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
+      <c r="J36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>160</v>
       </c>
@@ -2009,16 +2147,19 @@
         <v>163</v>
       </c>
       <c r="F37" s="1">
-        <v>7.04216581E8</v>
+        <v>704216581</v>
       </c>
       <c r="G37" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="I37" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
+      <c r="J37" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>164</v>
       </c>
@@ -2035,16 +2176,19 @@
         <v>167</v>
       </c>
       <c r="F38" s="1">
-        <v>7.30444721E8</v>
+        <v>730444721</v>
       </c>
       <c r="G38" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
+      <c r="J38" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>168</v>
       </c>
@@ -2061,16 +2205,19 @@
         <v>172</v>
       </c>
       <c r="F39" s="1">
-        <v>7.02350621E8</v>
+        <v>702350621</v>
       </c>
       <c r="G39" s="1">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
+      <c r="J39" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>173</v>
       </c>
@@ -2087,16 +2234,19 @@
         <v>175</v>
       </c>
       <c r="F40" s="1">
-        <v>7.30047902E8</v>
+        <v>730047902</v>
       </c>
       <c r="G40" s="1">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
+      <c r="J40" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>176</v>
       </c>
@@ -2113,16 +2263,19 @@
         <v>179</v>
       </c>
       <c r="F41" s="1">
-        <v>7.30084053E8</v>
+        <v>730084053</v>
       </c>
       <c r="G41" s="1">
-        <v>168.0</v>
+        <v>168</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
+      <c r="J41" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>180</v>
       </c>
@@ -2139,16 +2292,19 @@
         <v>184</v>
       </c>
       <c r="F42" s="1">
-        <v>7.30139149E8</v>
+        <v>730139149</v>
       </c>
       <c r="G42" s="1">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
+      <c r="J42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>185</v>
       </c>
@@ -2165,16 +2321,19 @@
         <v>188</v>
       </c>
       <c r="F43" s="1">
-        <v>7.09856816E8</v>
+        <v>709856816</v>
       </c>
       <c r="G43" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
+      <c r="J43" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>189</v>
       </c>
@@ -2191,16 +2350,19 @@
         <v>192</v>
       </c>
       <c r="F44" s="1">
-        <v>7.01875776E8</v>
+        <v>701875776</v>
       </c>
       <c r="G44" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
+      <c r="J44" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>193</v>
       </c>
@@ -2217,16 +2379,19 @@
         <v>196</v>
       </c>
       <c r="F45" s="1">
-        <v>7.06390995E8</v>
+        <v>706390995</v>
       </c>
       <c r="G45" s="1">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="I45" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
+      <c r="J45" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>197</v>
       </c>
@@ -2243,20 +2408,23 @@
         <v>201</v>
       </c>
       <c r="F46" s="1">
-        <v>7.30374691E8</v>
+        <v>730374691</v>
       </c>
       <c r="G46" s="1">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
+      <c r="J46" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>203</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -2269,16 +2437,19 @@
         <v>11</v>
       </c>
       <c r="F47" s="1">
-        <v>7.20422374E8</v>
+        <v>720422374</v>
       </c>
       <c r="G47" s="1">
-        <v>166.0</v>
+        <v>166</v>
       </c>
       <c r="I47" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
+      <c r="J47" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>206</v>
       </c>
@@ -2295,16 +2466,19 @@
         <v>208</v>
       </c>
       <c r="F48" s="1">
-        <v>7.04225848E8</v>
+        <v>704225848</v>
       </c>
       <c r="G48" s="1">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
+      <c r="J48" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>209</v>
       </c>
@@ -2321,16 +2495,19 @@
         <v>212</v>
       </c>
       <c r="F49" s="1">
-        <v>7.1381178E8</v>
+        <v>713811780</v>
       </c>
       <c r="G49" s="1">
-        <v>132.0</v>
+        <v>132</v>
       </c>
       <c r="I49" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
+      <c r="J49" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>213</v>
       </c>
@@ -2347,16 +2524,19 @@
         <v>216</v>
       </c>
       <c r="F50" s="1">
-        <v>7.04313363E8</v>
+        <v>704313363</v>
       </c>
       <c r="G50" s="1">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
+      <c r="J50" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>217</v>
       </c>
@@ -2373,16 +2553,19 @@
         <v>221</v>
       </c>
       <c r="F51" s="1">
-        <v>7.02502169E8</v>
+        <v>702502169</v>
       </c>
       <c r="G51" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
+      <c r="J51" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>222</v>
       </c>
@@ -2399,10 +2582,10 @@
         <v>226</v>
       </c>
       <c r="F52" s="1">
-        <v>7.10985109E8</v>
+        <v>710985109</v>
       </c>
       <c r="G52" s="1">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="H52" s="1" t="b">
         <v>1</v>
@@ -2410,8 +2593,11 @@
       <c r="I52" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
+      <c r="J52" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>227</v>
       </c>
@@ -2428,16 +2614,19 @@
         <v>231</v>
       </c>
       <c r="F53" s="1">
-        <v>7.10231503E8</v>
+        <v>710231503</v>
       </c>
       <c r="G53" s="1">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
+      <c r="J53" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>232</v>
       </c>
@@ -2454,16 +2643,19 @@
         <v>236</v>
       </c>
       <c r="F54" s="1">
-        <v>7.02025507E8</v>
+        <v>702025507</v>
       </c>
       <c r="G54" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="I54" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
+      <c r="J54" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>237</v>
       </c>
@@ -2477,16 +2669,19 @@
         <v>240</v>
       </c>
       <c r="F55" s="1">
-        <v>7.05423928E8</v>
+        <v>705423928</v>
       </c>
       <c r="G55" s="1">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="I55" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
+      <c r="J55" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>241</v>
       </c>
@@ -2503,16 +2698,19 @@
         <v>244</v>
       </c>
       <c r="F56" s="1">
-        <v>7.00599204E8</v>
+        <v>700599204</v>
       </c>
       <c r="G56" s="1">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="I56" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
+      <c r="J56" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>245</v>
       </c>
@@ -2529,10 +2727,10 @@
         <v>249</v>
       </c>
       <c r="F57" s="1">
-        <v>7.30445086E8</v>
+        <v>730445086</v>
       </c>
       <c r="G57" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H57" s="1" t="b">
         <v>1</v>
@@ -2540,8 +2738,11 @@
       <c r="I57" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
+      <c r="J57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>250</v>
       </c>
@@ -2558,958 +2759,961 @@
         <v>253</v>
       </c>
       <c r="F58" s="1">
-        <v>7.14750042E8</v>
+        <v>714750042</v>
       </c>
       <c r="G58" s="1">
-        <v>164.0</v>
+        <v>164</v>
       </c>
       <c r="I58" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+      <c r="J58" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>